<commit_message>
Small fixes/changes in the json example of the standaard
</commit_message>
<xml_diff>
--- a/files/Stembureaus Open Data Standaard 1.6 - Europese Parlementsverkiezingen 2024 voorbeeld.xlsx
+++ b/files/Stembureaus Open Data Standaard 1.6 - Europese Parlementsverkiezingen 2024 voorbeeld.xlsx
@@ -911,14 +911,7 @@
     <t xml:space="preserve">De standaard is beschreven als platte tabel, zodat de data op te slaan is als CSV- of spreadsheet-bestand. De standaard bevat echter soms geneste informatie. Daar wordt mee omgegaan door informatie te dupliceren over meerdere kolommen (zie bv. de ‘Openingstijd’- en ‘Sluitingstijd’-attributen). JSON-bestanden zijn iets complexer, maar kunnen beter omgaan met geneste informatie. De in deze standaard beschreven informatie kan daarom ook als JSON-bestand opgeslagen worden. Hieronder staat een voorbeeld van hoe dit eruit ziet voor de attributen (de metadata spreekt voor zich aangezien daar geen geneste informatie in voorkomt). Meerdere locaties worden dan ondergebracht onder de lijst ‘Locaties’ en meerdere openingstijden onder de lijst ‘Openingstijden’.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FF000000"/>
-        <rFont val="arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[
+    <t xml:space="preserve">[
   {
     "Gemeente": "'s-Gravenhage",
     "CBS gemeentecode": "GM0518",
@@ -928,25 +921,7 @@
     "Locaties": [
         {
             "Gebruiksdoel van het gebouw": "Kantoor",
-            "Website locatie": "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://www.denhaag.nl/nl/contact-met-de-gemeente/stadhuis-den-haag/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FF000000"/>
-        <rFont val="arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">",
+            "Website locatie": "https://www.denhaag.nl/nl/contact-met-de-gemeente/stadhuis-den-haag/",
             "Wijknaam": "Centrum",
             "CBS Wijknummer": "WK051828",
             "Buurtnaam": "Kortenbos",
@@ -965,8 +940,7 @@
             "Longitude": 4.3166395,
             "Openingstijden": [
                 {"Openingstijd": "2024-06-06T10:00:00", "Sluitingstijd": "2024-06-06T13:00:00"},
-                {"Openingstijd": "2024-06-06T14:00:00", "Sluitingstijd": "2024-06-06T21:00:00"},
-                ...
+                {"Openingstijd": "2024-06-06T14:00:00", "Sluitingstijd": "2024-06-06T21:00:00"}
             ],
             "Toegankelijk voor mensen met een lichamelijke beperking": "ja",
             "Toegankelijke ov-halte": "ja",
@@ -980,21 +954,18 @@
             "Gebarentalige stembureauleden (NGT)": "ja",
             "Akoestiek geschikt voor slechthorenden": "ja",
             "Prikkelarm": "ja",
-            "Extra toegankelijkheidsinformatie: "Dit stembureau is ingericht voor kwetsbare mensen, stembureau is volledig toegankelijk voor mensen met een lichamelijke beperking er is echter geen gehandicaptenparkeerplaats, gebarentolk op locatie (NGT) is aanwezig van 10:00-12:00 en 16:00-18:00, oefenstembureau", 
+            "Extra toegankelijkheidsinformatie": "Dit stembureau is ingericht voor kwetsbare mensen, stembureau is volledig toegankelijk voor mensen met een lichamelijke beperking er is echter geen gehandicaptenparkeerplaats, gebarentolk op locatie (NGT) is aanwezig van 10:00-12:00 en 16:00-18:00, oefenstembureau", 
             "Overige informatie": "",
             "Tellocatie": "ja"
-        },
-        ...
+        }
     ],
     "Kieskring ID": "1",
     "Hoofdstembureau": "'s-Gravenhage",
     "Contactgegevens gemeente": "Unit Verkiezingen, verkiezingen@denhaag.nl 070-3534488 Gemeente Den Haag Publiekszaken/Unit Verkiezingen Postbus 84008 2508 AA Den Haag",
     "Verkiezingswebsite gemeente": "https://www.stembureausindenhaag.nl/",
     "Verkiezingen": "waterschapsverkiezingen voor Delfland"
-  },
-  ...
+  }
 ]</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -1006,7 +977,7 @@
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1195,12 +1166,6 @@
       <name val="arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -3967,7 +3932,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="442.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="420.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="56" t="s">
         <v>205</v>
       </c>

</xml_diff>

<commit_message>
Make sure the standard spreadsheets have their tabs saved showing all columns
</commit_message>
<xml_diff>
--- a/files/Stembureaus Open Data Standaard 1.6 - Europese Parlementsverkiezingen 2024 voorbeeld.xlsx
+++ b/files/Stembureaus Open Data Standaard 1.6 - Europese Parlementsverkiezingen 2024 voorbeeld.xlsx
@@ -1873,8 +1873,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1890,7 +1890,7 @@
   <dimension ref="A1:AMJ50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
@@ -3283,8 +3283,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3300,7 +3300,7 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
@@ -3902,11 +3902,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
@@ -3939,11 +3939,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>